<commit_message>
Add more unfinished graphs
</commit_message>
<xml_diff>
--- a/lab3/Experiment 3/vSweep.xlsx
+++ b/lab3/Experiment 3/vSweep.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="vSweep" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1180,11 +1180,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71444160"/>
-        <c:axId val="71444736"/>
+        <c:axId val="511130368"/>
+        <c:axId val="516856576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71444160"/>
+        <c:axId val="511130368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,12 +1223,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71444736"/>
+        <c:crossAx val="516856576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71444736"/>
+        <c:axId val="516856576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71444160"/>
+        <c:crossAx val="511130368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1906,7 +1906,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,11 +1968,11 @@
         <v>0.05</v>
       </c>
       <c r="E4">
-        <f>B4-B3</f>
+        <f t="shared" ref="E4:E35" si="1">B4-B3</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F67" si="1">E4/D4</f>
+        <f t="shared" ref="F4:F67" si="2">E4/D4</f>
         <v>0</v>
       </c>
     </row>
@@ -1988,11 +1988,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E5">
-        <f>B5-B4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2008,11 +2008,11 @@
         <v>5.0000000000000017E-2</v>
       </c>
       <c r="E6">
-        <f>B6-B5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2028,11 +2028,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E7">
-        <f>B7-B6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2048,11 +2048,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E8">
-        <f>B8-B7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2068,11 +2068,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E9">
-        <f>B9-B8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2088,11 +2088,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E10">
-        <f>B10-B9</f>
+        <f t="shared" si="1"/>
         <v>1E-3</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9999999999999983E-2</v>
       </c>
     </row>
@@ -2108,11 +2108,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E11">
-        <f>B11-B10</f>
+        <f t="shared" si="1"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0000000000000012E-2</v>
       </c>
     </row>
@@ -2128,11 +2128,11 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="E12">
-        <f>B12-B11</f>
+        <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26000000000000006</v>
       </c>
     </row>
@@ -2148,11 +2148,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E13">
-        <f>B13-B12</f>
+        <f t="shared" si="1"/>
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.51999999999999946</v>
       </c>
     </row>
@@ -2168,11 +2168,11 @@
         <v>4.9999999999999933E-2</v>
       </c>
       <c r="E14">
-        <f>B14-B13</f>
+        <f t="shared" si="1"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70000000000000095</v>
       </c>
     </row>
@@ -2188,11 +2188,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E15">
-        <f>B15-B14</f>
+        <f t="shared" si="1"/>
         <v>3.8999999999999993E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.77999999999999914</v>
       </c>
     </row>
@@ -2208,11 +2208,11 @@
         <v>4.9999999999999933E-2</v>
       </c>
       <c r="E16">
-        <f>B16-B15</f>
+        <f t="shared" si="1"/>
         <v>4.200000000000001E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8400000000000013</v>
       </c>
     </row>
@@ -2228,11 +2228,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E17">
-        <f>B17-B16</f>
+        <f t="shared" si="1"/>
         <v>4.2999999999999983E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85999999999999888</v>
       </c>
     </row>
@@ -2248,11 +2248,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E18">
-        <f>B18-B17</f>
+        <f t="shared" si="1"/>
         <v>4.5000000000000012E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89999999999999947</v>
       </c>
     </row>
@@ -2268,11 +2268,11 @@
         <v>4.9999999999999933E-2</v>
       </c>
       <c r="E19">
-        <f>B19-B18</f>
+        <f t="shared" si="1"/>
         <v>4.4999999999999984E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90000000000000091</v>
       </c>
     </row>
@@ -2288,11 +2288,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E20">
-        <f>B20-B19</f>
+        <f t="shared" si="1"/>
         <v>4.6000000000000041E-2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92</v>
       </c>
     </row>
@@ -2308,11 +2308,11 @@
         <v>4.9999999999999933E-2</v>
       </c>
       <c r="E21">
-        <f>B21-B20</f>
+        <f t="shared" si="1"/>
         <v>4.5999999999999985E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92000000000000093</v>
       </c>
     </row>
@@ -2328,11 +2328,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E22">
-        <f>B22-B21</f>
+        <f t="shared" si="1"/>
         <v>4.7999999999999987E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999885</v>
       </c>
     </row>
@@ -2348,11 +2348,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E23">
-        <f>B23-B22</f>
+        <f t="shared" si="1"/>
         <v>4.7999999999999987E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999885</v>
       </c>
     </row>
@@ -2368,11 +2368,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E24">
-        <f>B24-B23</f>
+        <f t="shared" si="1"/>
         <v>4.7000000000000042E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
     </row>
@@ -2388,11 +2388,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E25">
-        <f>B25-B24</f>
+        <f t="shared" si="1"/>
         <v>4.7999999999999932E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96000000000000207</v>
       </c>
     </row>
@@ -2408,11 +2408,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E26">
-        <f>B26-B25</f>
+        <f t="shared" si="1"/>
         <v>4.7000000000000042E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
     </row>
@@ -2428,11 +2428,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E27">
-        <f>B27-B26</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2448,11 +2448,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E28">
-        <f>B28-B27</f>
+        <f t="shared" si="1"/>
         <v>4.7999999999999932E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999774</v>
       </c>
     </row>
@@ -2468,11 +2468,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E29">
-        <f>B29-B28</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2488,11 +2488,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E30">
-        <f>B30-B29</f>
+        <f t="shared" si="1"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98000000000000209</v>
       </c>
     </row>
@@ -2508,11 +2508,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E31">
-        <f>B31-B30</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2528,11 +2528,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E32">
-        <f>B32-B31</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2548,11 +2548,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E33">
-        <f>B33-B32</f>
+        <f t="shared" si="1"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97999999999999776</v>
       </c>
     </row>
@@ -2568,11 +2568,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E34">
-        <f>B34-B33</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2588,11 +2588,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E35">
-        <f>B35-B34</f>
+        <f t="shared" si="1"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98000000000000209</v>
       </c>
     </row>
@@ -2608,11 +2608,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E36">
-        <f>B36-B35</f>
+        <f t="shared" ref="E36:E67" si="3">B36-B35</f>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2628,11 +2628,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E37">
-        <f>B37-B36</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2648,11 +2648,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E38">
-        <f>B38-B37</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2668,11 +2668,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E39">
-        <f>B39-B38</f>
+        <f t="shared" si="3"/>
         <v>4.7999999999999821E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999552</v>
       </c>
     </row>
@@ -2688,11 +2688,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E40">
-        <f>B40-B39</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -2708,11 +2708,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E41">
-        <f>B41-B40</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2728,11 +2728,11 @@
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="E42">
-        <f>B42-B41</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
     </row>
@@ -2748,11 +2748,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E43">
-        <f>B43-B42</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -2768,11 +2768,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E44">
-        <f>B44-B43</f>
+        <f t="shared" si="3"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97999999999999343</v>
       </c>
     </row>
@@ -2788,11 +2788,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E45">
-        <f>B45-B44</f>
+        <f t="shared" si="3"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98000000000000209</v>
       </c>
     </row>
@@ -2808,11 +2808,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E46">
-        <f>B46-B45</f>
+        <f t="shared" si="3"/>
         <v>4.9000000000000155E-2</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97999999999999787</v>
       </c>
     </row>
@@ -2828,11 +2828,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E47">
-        <f>B47-B46</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2848,11 +2848,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E48">
-        <f>B48-B47</f>
+        <f t="shared" si="3"/>
         <v>4.9000000000000155E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98000000000000653</v>
       </c>
     </row>
@@ -2868,11 +2868,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E49">
-        <f>B49-B48</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -2888,11 +2888,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E50">
-        <f>B50-B49</f>
+        <f t="shared" si="3"/>
         <v>4.7999999999999821E-2</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999985</v>
       </c>
     </row>
@@ -2908,11 +2908,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E51">
-        <f>B51-B50</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -2928,11 +2928,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E52">
-        <f>B52-B51</f>
+        <f t="shared" si="3"/>
         <v>4.8999999999999932E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98000000000000209</v>
       </c>
     </row>
@@ -2948,11 +2948,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E53">
-        <f>B53-B52</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000044</v>
       </c>
     </row>
@@ -2968,11 +2968,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E54">
-        <f>B54-B53</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -2988,11 +2988,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E55">
-        <f>B55-B54</f>
+        <f t="shared" si="3"/>
         <v>5.9999999999999831E-2</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2000000000000008</v>
       </c>
     </row>
@@ -3008,11 +3008,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E56">
-        <f>B56-B55</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3028,11 +3028,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E57">
-        <f>B57-B56</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3048,11 +3048,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E58">
-        <f>B58-B57</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3068,11 +3068,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E59">
-        <f>B59-B58</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99999999999999112</v>
       </c>
     </row>
@@ -3088,11 +3088,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E60">
-        <f>B60-B59</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3108,11 +3108,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E61">
-        <f>B61-B60</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99999999999999112</v>
       </c>
     </row>
@@ -3128,11 +3128,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E62">
-        <f>B62-B61</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3148,11 +3148,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E63">
-        <f>B63-B62</f>
+        <f t="shared" si="3"/>
         <v>5.2000000000000046E-2</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0400000000000047</v>
       </c>
     </row>
@@ -3168,11 +3168,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E64">
-        <f>B64-B63</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3188,11 +3188,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E65">
-        <f>B65-B64</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3208,11 +3208,11 @@
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E66">
-        <f>B66-B65</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3228,11 +3228,11 @@
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E67">
-        <f>B67-B66</f>
+        <f t="shared" si="3"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3244,15 +3244,15 @@
         <v>2.6840000000000002</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:D102" si="2">A68-A67</f>
+        <f t="shared" ref="D68:D102" si="4">A68-A67</f>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E68">
-        <f>B68-B67</f>
+        <f t="shared" ref="E68:E102" si="5">B68-B67</f>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F102" si="3">E68/D68</f>
+        <f t="shared" ref="F68:F102" si="6">E68/D68</f>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3264,15 +3264,15 @@
         <v>2.734</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E69">
-        <f>B69-B68</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99999999999999112</v>
       </c>
     </row>
@@ -3284,15 +3284,15 @@
         <v>2.782</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E70">
-        <f>B70-B69</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3304,15 +3304,15 @@
         <v>2.83</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E71">
-        <f>B71-B70</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3324,15 +3324,15 @@
         <v>2.88</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E72">
-        <f>B72-B71</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3344,15 +3344,15 @@
         <v>2.93</v>
       </c>
       <c r="D73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E73">
-        <f>B73-B72</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3364,15 +3364,15 @@
         <v>2.9780000000000002</v>
       </c>
       <c r="D74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E74">
-        <f>B74-B73</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3384,15 +3384,15 @@
         <v>3.028</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E75">
-        <f>B75-B74</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3404,15 +3404,15 @@
         <v>3.0760000000000001</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E76">
-        <f>B76-B75</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.95999999999999575</v>
       </c>
     </row>
@@ -3424,15 +3424,15 @@
         <v>3.1259999999999999</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E77">
-        <f>B77-B76</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3444,15 +3444,15 @@
         <v>3.1739999999999999</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E78">
-        <f>B78-B77</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3464,15 +3464,15 @@
         <v>3.2240000000000002</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E79">
-        <f>B79-B78</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3484,15 +3484,15 @@
         <v>3.2719999999999998</v>
       </c>
       <c r="D80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E80">
-        <f>B80-B79</f>
+        <f t="shared" si="5"/>
         <v>4.7999999999999599E-2</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.95999999999999541</v>
       </c>
     </row>
@@ -3504,15 +3504,15 @@
         <v>3.3180000000000001</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="E81">
-        <f>B81-B80</f>
+        <f t="shared" si="5"/>
         <v>4.6000000000000263E-2</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.92000000000000037</v>
       </c>
     </row>
@@ -3524,15 +3524,15 @@
         <v>3.3679999999999999</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E82">
-        <f>B82-B81</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3544,15 +3544,15 @@
         <v>3.4180000000000001</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E83">
-        <f>B83-B82</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3564,15 +3564,15 @@
         <v>3.468</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E84">
-        <f>B84-B83</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3584,15 +3584,15 @@
         <v>3.5179999999999998</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000711E-2</v>
       </c>
       <c r="E85">
-        <f>B85-B84</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99999999999998224</v>
       </c>
     </row>
@@ -3604,15 +3604,15 @@
         <v>3.5659999999999998</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E86">
-        <f>B86-B85</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3624,15 +3624,15 @@
         <v>3.6160000000000001</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E87">
-        <f>B87-B86</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3644,15 +3644,15 @@
         <v>3.6640000000000001</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E88">
-        <f>B88-B87</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3664,15 +3664,15 @@
         <v>3.714</v>
       </c>
       <c r="D89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E89">
-        <f>B89-B88</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3684,15 +3684,15 @@
         <v>3.762</v>
       </c>
       <c r="D90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000711E-2</v>
       </c>
       <c r="E90">
-        <f>B90-B89</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.9599999999999872</v>
       </c>
     </row>
@@ -3704,15 +3704,15 @@
         <v>3.81</v>
       </c>
       <c r="D91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E91">
-        <f>B91-B90</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3724,15 +3724,15 @@
         <v>3.86</v>
       </c>
       <c r="D92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E92">
-        <f>B92-B91</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="F92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3744,15 +3744,15 @@
         <v>3.9079999999999999</v>
       </c>
       <c r="D93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E93">
-        <f>B93-B92</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3764,15 +3764,15 @@
         <v>3.9580000000000002</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E94">
-        <f>B94-B93</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000266E-2</v>
       </c>
       <c r="F94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000089</v>
       </c>
     </row>
@@ -3784,15 +3784,15 @@
         <v>4.0060000000000002</v>
       </c>
       <c r="D95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000711E-2</v>
       </c>
       <c r="E95">
-        <f>B95-B94</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.9599999999999872</v>
       </c>
     </row>
@@ -3804,15 +3804,15 @@
         <v>4.0540000000000003</v>
       </c>
       <c r="D96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E96">
-        <f>B96-B95</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3824,15 +3824,15 @@
         <v>4.1020000000000003</v>
       </c>
       <c r="D97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E97">
-        <f>B97-B96</f>
+        <f t="shared" si="5"/>
         <v>4.8000000000000043E-2</v>
       </c>
       <c r="F97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.96000000000000429</v>
       </c>
     </row>
@@ -3844,15 +3844,15 @@
         <v>4.1159999999999997</v>
       </c>
       <c r="D98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E98">
-        <f>B98-B97</f>
+        <f t="shared" si="5"/>
         <v>1.3999999999999346E-2</v>
       </c>
       <c r="F98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.27999999999998793</v>
       </c>
     </row>
@@ -3864,15 +3864,15 @@
         <v>4.1159999999999997</v>
       </c>
       <c r="D99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E99">
-        <f>B99-B98</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3884,15 +3884,15 @@
         <v>4.1159999999999997</v>
       </c>
       <c r="D100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000711E-2</v>
       </c>
       <c r="E100">
-        <f>B100-B99</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3904,15 +3904,15 @@
         <v>4.1159999999999997</v>
       </c>
       <c r="D101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E101">
-        <f>B101-B100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3924,15 +3924,15 @@
         <v>4.1159999999999997</v>
       </c>
       <c r="D102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
       <c r="E102">
-        <f>B102-B101</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add lab5 - brad code
</commit_message>
<xml_diff>
--- a/lab3/Experiment 3/vSweep.xlsx
+++ b/lab3/Experiment 3/vSweep.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="vSweep" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -663,7 +666,7 @@
                     </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = 0.9773 - 0.5449
+                      <a:t>y = 0.9773x(V) - 0.5449
 R² = 0.9999</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US" sz="1600"/>
@@ -1181,11 +1184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45733504"/>
-        <c:axId val="45734080"/>
+        <c:axId val="555896192"/>
+        <c:axId val="555897920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45733504"/>
+        <c:axId val="555896192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,12 +1227,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45734080"/>
+        <c:crossAx val="555897920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45734080"/>
+        <c:axId val="555897920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,7 +1272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45733504"/>
+        <c:crossAx val="555896192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2021,17 +2024,24 @@
                   <c:y val="-0.12935566417346311"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400"/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 0.0052x(V) + 0.96
+R² = 0.0735</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -2515,11 +2525,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46690816"/>
-        <c:axId val="46691968"/>
+        <c:axId val="524155072"/>
+        <c:axId val="576151552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46690816"/>
+        <c:axId val="524155072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,12 +2568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46691968"/>
+        <c:crossAx val="576151552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46691968"/>
+        <c:axId val="576151552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,7 +2618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46690816"/>
+        <c:crossAx val="524155072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2725,6 +2735,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="VTC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3578,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5619,8 +5642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>